<commit_message>
envio de imagem PM
</commit_message>
<xml_diff>
--- a/cad_user/LOT14IMEIGUARD.xlsx
+++ b/cad_user/LOT14IMEIGUARD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\deac_ti_sw\Users\DEAC_TI_SERVER\Desktop\IMEIGUARD\cad_user\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DEAC_TI_SW\Users\DEAC_TI_SERVER\Desktop\IMEIGUARD\cad_user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE7A3BB-27E2-4C95-B832-499FF1BE67CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014C61CA-E32D-4A43-83F3-18A48446D369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respostas ao formulário 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -177,6 +177,45 @@
   </si>
   <si>
     <t>PAP</t>
+  </si>
+  <si>
+    <t>direito.ariclessilva@gmail.com</t>
+  </si>
+  <si>
+    <t>MPC</t>
+  </si>
+  <si>
+    <t>jacksonwla@gmail.com</t>
+  </si>
+  <si>
+    <t>JACKSON WENDELL LOPES DE ALMEIDA</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>ROTAM</t>
+  </si>
+  <si>
+    <t>jefferson.rodrisouza@gmail.com</t>
+  </si>
+  <si>
+    <t>jefferson.souza@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>ARICLES DE SOUSA SILVA</t>
+  </si>
+  <si>
+    <t>JEFFERSON RODRIGUES SOUZA</t>
+  </si>
+  <si>
+    <t>SUPERINTENDENCIA CASTANHAL, 3 RISP</t>
+  </si>
+  <si>
+    <t>DELEGACIA DE BENFICA</t>
+  </si>
+  <si>
+    <t>SGT</t>
   </si>
 </sst>
 </file>
@@ -516,7 +555,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD24"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="A11:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -855,9 +894,102 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>45485.94604166667</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="6">
+        <v>5453003</v>
+      </c>
+      <c r="E11" s="6">
+        <v>17116414215</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>45488.699837962966</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="6">
+        <v>541930761</v>
+      </c>
+      <c r="E12" s="6">
+        <v>72273275234</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>45488.726354166669</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="6">
+        <v>4219631</v>
+      </c>
+      <c r="E13" s="5">
+        <v>2041287225</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="14" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -935,5 +1067,6 @@
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
atualizacao de usuarios confirmados
</commit_message>
<xml_diff>
--- a/cad_user/LOT14IMEIGUARD.xlsx
+++ b/cad_user/LOT14IMEIGUARD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DEAC_TI_SW\Users\DEAC_TI_SERVER\Desktop\IMEIGUARD\cad_user\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\deac_ti_sw\Users\DEAC_TI_SERVER\Desktop\IMEIGUARD\cad_user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014C61CA-E32D-4A43-83F3-18A48446D369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FD4921-D0A1-4492-AE58-A4F2C32E0760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="78">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -216,6 +216,60 @@
   </si>
   <si>
     <t>SGT</t>
+  </si>
+  <si>
+    <t>melojunior3103@gmail.com</t>
+  </si>
+  <si>
+    <t>DPM SRM DELEGACIA DE POLICIA DO ICUI-GUAJARA</t>
+  </si>
+  <si>
+    <t>alexsandrowidmar@gmail.com</t>
+  </si>
+  <si>
+    <t>alexsandro.widmar@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>andradefabiohot@gmail.com</t>
+  </si>
+  <si>
+    <t>FABIO DE ANDRADE PEREIRA</t>
+  </si>
+  <si>
+    <t>ANANINDEUA</t>
+  </si>
+  <si>
+    <t>fabio.pereira@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>hiagolima.adv@gmail.com</t>
+  </si>
+  <si>
+    <t>hiago.ferreira@poIiciaciviI.pa.gov.br</t>
+  </si>
+  <si>
+    <t>kamar.alves@gmail.com</t>
+  </si>
+  <si>
+    <t>kamar.barbosa@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>SECCIONAL DA CIDADE NOVA</t>
+  </si>
+  <si>
+    <t>DELEGACIA DE CAPANEMA-PA</t>
+  </si>
+  <si>
+    <t>ALEXSANDRO WIDMAR</t>
+  </si>
+  <si>
+    <t>HIAGO LIMA FERREIRA</t>
+  </si>
+  <si>
+    <t>KAMAR ALVES DA SILVA BARBOSA</t>
+  </si>
+  <si>
+    <t>NELSON MONTEIRO DE MELO JUNIOR</t>
   </si>
 </sst>
 </file>
@@ -311,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -333,6 +387,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,11 +615,11 @@
   <sheetPr codeName="Planilha1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O69"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J13" sqref="A11:J13"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -990,79 +1054,197 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="5:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="5:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="5:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="5:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="5:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="5:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="5:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="5:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="5:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="5:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="5:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="5:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="5:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E61" s="1"/>
-    </row>
-    <row r="62" spans="5:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="5:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E63" s="1"/>
-    </row>
-    <row r="64" spans="5:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E64" s="1"/>
-    </row>
-    <row r="65" spans="5:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E65" s="1"/>
-    </row>
-    <row r="66" spans="5:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E66" s="1"/>
-    </row>
-    <row r="67" spans="5:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E67" s="1"/>
-    </row>
-    <row r="68" spans="5:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" spans="5:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E69" s="1"/>
+    <row r="14" spans="1:15" s="12" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>45489.523923611108</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="10">
+        <v>5331501</v>
+      </c>
+      <c r="E14" s="10">
+        <v>21852170204</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>45489.581886574073</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="6">
+        <v>5940474</v>
+      </c>
+      <c r="E15" s="5">
+        <v>2060056012</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>45489.725960648146</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="6">
+        <v>5913936</v>
+      </c>
+      <c r="E16" s="5">
+        <v>3295607435</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>45490.347418981481</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="6">
+        <v>5967000</v>
+      </c>
+      <c r="E17" s="5">
+        <v>17348017889</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>45490.468032407407</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="6">
+        <v>5966792</v>
+      </c>
+      <c r="E18" s="5">
+        <v>4671853361</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E32" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>